<commit_message>
Got basic API call working
</commit_message>
<xml_diff>
--- a/Documentation/Tasks.xlsx
+++ b/Documentation/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\PowerGrid\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AF017C-47A5-4347-897A-61546BEE630A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64AD0CD-E495-4CB3-A2C7-047DFE7D556E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9330" xr2:uid="{28DC5C9A-E163-4544-AAC7-BC936B05F4D3}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Task</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t>Create Domain files</t>
+  </si>
+  <si>
+    <t>Get Api call working</t>
+  </si>
+  <si>
+    <t>Fix CORS</t>
   </si>
 </sst>
 </file>
@@ -425,16 +431,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D0AE0CB-64F7-4B1F-BE23-1007490FE6E8}">
-  <dimension ref="B1:D6"/>
+  <dimension ref="B1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="82.42578125" customWidth="1"/>
-    <col min="3" max="3" width="67" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -490,6 +496,19 @@
       </c>
       <c r="D6" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Mock server data. Add Gamestate domain object. Websocket working. Some work on pushing gamestate to client
</commit_message>
<xml_diff>
--- a/Documentation/Tasks.xlsx
+++ b/Documentation/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\PowerGrid\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64AD0CD-E495-4CB3-A2C7-047DFE7D556E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A39B3B-1F66-4B9D-A30E-37C84D6DFE8B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9330" xr2:uid="{28DC5C9A-E163-4544-AAC7-BC936B05F4D3}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>Task</t>
   </si>
@@ -61,13 +61,22 @@
     <t>In Progress</t>
   </si>
   <si>
-    <t>Create Domain files</t>
-  </si>
-  <si>
     <t>Get Api call working</t>
   </si>
   <si>
     <t>Fix CORS</t>
+  </si>
+  <si>
+    <t>Create Domain files Player and Card</t>
+  </si>
+  <si>
+    <t>Create domain file Resources</t>
+  </si>
+  <si>
+    <t>Learn how to make request that keeps listening</t>
+  </si>
+  <si>
+    <t>Create domain gamestate object</t>
   </si>
 </sst>
 </file>
@@ -431,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D0AE0CB-64F7-4B1F-BE23-1007490FE6E8}">
-  <dimension ref="B1:D8"/>
+  <dimension ref="B1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,15 +501,15 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
@@ -508,7 +517,28 @@
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed css alignment issue
</commit_message>
<xml_diff>
--- a/Documentation/Tasks.xlsx
+++ b/Documentation/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\PowerGrid\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A39B3B-1F66-4B9D-A30E-37C84D6DFE8B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4C8579-0A1A-4FAC-98E5-600144129BCE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9330" xr2:uid="{28DC5C9A-E163-4544-AAC7-BC936B05F4D3}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>Task</t>
   </si>
@@ -77,6 +77,19 @@
   </si>
   <si>
     <t>Create domain gamestate object</t>
+  </si>
+  <si>
+    <t>Add Resource market domain classes</t>
+  </si>
+  <si>
+    <t>Refactor: remove PropertyName for domain classes in C#. Use this
+(https://stackoverflow.com/questions/36883970/return-json-with-lower-case-first-letter-of-property-names)</t>
+  </si>
+  <si>
+    <t>To be done</t>
+  </si>
+  <si>
+    <t>Bugs: Figure out css alignment</t>
   </si>
 </sst>
 </file>
@@ -112,8 +125,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D0AE0CB-64F7-4B1F-BE23-1007490FE6E8}">
-  <dimension ref="B1:D11"/>
+  <dimension ref="B1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,6 +543,9 @@
       <c r="B9" t="s">
         <v>13</v>
       </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -539,6 +558,27 @@
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add api command prototype to angular app
</commit_message>
<xml_diff>
--- a/Documentation/Tasks.xlsx
+++ b/Documentation/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\PowerGrid\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4C8579-0A1A-4FAC-98E5-600144129BCE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A9353B-3CBC-401F-B585-B2F59D6172EF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9330" xr2:uid="{28DC5C9A-E163-4544-AAC7-BC936B05F4D3}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>Task</t>
   </si>
@@ -90,6 +90,30 @@
   </si>
   <si>
     <t>Bugs: Figure out css alignment</t>
+  </si>
+  <si>
+    <t>Refactor components such that we have a gamestate component</t>
+  </si>
+  <si>
+    <t>API Function to buy Card</t>
+  </si>
+  <si>
+    <t>API Function to buy Resource</t>
+  </si>
+  <si>
+    <t>API Function to buy Generators</t>
+  </si>
+  <si>
+    <t>Add Map Component</t>
+  </si>
+  <si>
+    <t>Add Domain classes for maps</t>
+  </si>
+  <si>
+    <t>Need to cleanup angular services</t>
+  </si>
+  <si>
+    <t>Implement the constant gamestate</t>
   </si>
 </sst>
 </file>
@@ -456,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D0AE0CB-64F7-4B1F-BE23-1007490FE6E8}">
-  <dimension ref="B1:D14"/>
+  <dimension ref="B1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,6 +603,52 @@
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>